<commit_message>
algun mensaje de lo que voy a subir
</commit_message>
<xml_diff>
--- a/src/ranger/Ranger OB_analisis.xlsx
+++ b/src/ranger/Ranger OB_analisis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Facultad\Maestria DM\Expecializacion\DMEyF\Carpetas\labo\src\ranger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B352A17C-0335-43F5-86A6-B659C4977D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BFF73B-1C00-42E6-BA85-E4B1DD6740E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7111379B-5499-46D5-B7B6-9B71E12DE324}"/>
   </bookViews>
@@ -17,61 +17,23 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$76</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$2:$C$71</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$I$10:$I$71</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$I$14:$I$71</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$I$19:$I$71</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$I$21:$I$71</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$I$24:$I$70</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$I$24:$I$71</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$I$24:$I$72</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$I$24:$I$81</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$I$2:$I$20</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$I$2:$I$22</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$2:$C$80</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$I$2:$I$25</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$I$2:$I$28</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$I$2:$I$29</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$I$2:$I$32</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$I$2:$I$34</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$I$2:$I$35</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$I$2:$I$36</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$I$2:$I$43</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$I$2:$I$70</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$I$2:$I$71</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$I$7:$I$71</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$I$1</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$I$2:$I$14</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$I$2:$I$15</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$I$2:$I$17</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$I$2:$I$23</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$I$2:$I$29</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$I$2:$I$3</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$I$2:$I$33</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$I$2:$I$43</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$2:$D$71</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$I$2:$I$5</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$I$2:$I$57</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$I$2:$I$6</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$I$2:$I$61</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$I$2:$I$64</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$I$2:$I$66</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$I$2:$I$70</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$I$2:$I$71</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Sheet1!$I$2:$I$72</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">Sheet1!$I$2:$I$8</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$2:$D$84</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">Sheet1!$E$2:$E$71</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">Sheet1!$B$2:$B$71</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$B$2:$B$72</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$E$2:$E$71</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$E$2:$E$82</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$I$1</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$I$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$I$19:$I$104</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$2:$C$104</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$D$2:$D$103</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$D$2:$D$84</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$E$2:$E$104</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$E$2:$E$82</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$I$2:$I$104</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$I$2:$I$72</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$2:$B$104</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$I$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$I$24:$I$103</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$I$2:$I$103</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -94,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t>fecha</t>
   </si>
@@ -349,6 +311,72 @@
   </si>
   <si>
     <t>20220922 205217</t>
+  </si>
+  <si>
+    <t>20220922 210021</t>
+  </si>
+  <si>
+    <t>20220922 210245</t>
+  </si>
+  <si>
+    <t>20220922 211059</t>
+  </si>
+  <si>
+    <t>20220922 211526</t>
+  </si>
+  <si>
+    <t>20220922 211942</t>
+  </si>
+  <si>
+    <t>20220922 212913</t>
+  </si>
+  <si>
+    <t>20220922 213809</t>
+  </si>
+  <si>
+    <t>20220922 213854</t>
+  </si>
+  <si>
+    <t>20220922 214512</t>
+  </si>
+  <si>
+    <t>20220922 215214</t>
+  </si>
+  <si>
+    <t>20220922 215946</t>
+  </si>
+  <si>
+    <t>20220922 220726</t>
+  </si>
+  <si>
+    <t>20220922 221426</t>
+  </si>
+  <si>
+    <t>20220922 221609</t>
+  </si>
+  <si>
+    <t>20220922 222034</t>
+  </si>
+  <si>
+    <t>20220922 222428</t>
+  </si>
+  <si>
+    <t>20220922 222949</t>
+  </si>
+  <si>
+    <t>20220922 223608</t>
+  </si>
+  <si>
+    <t>20220922 224314</t>
+  </si>
+  <si>
+    <t>20220922 224654</t>
+  </si>
+  <si>
+    <t>20220922 224912</t>
+  </si>
+  <si>
+    <t>20220922 225745</t>
   </si>
 </sst>
 </file>
@@ -357,7 +385,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -418,12 +446,12 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -447,7 +475,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -458,7 +486,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{847F72E7-4E63-4CB2-982D-5A27621DA617}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.9</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>bin</cx:v>
             </cx:txData>
           </cx:tx>
@@ -493,7 +521,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.48</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -504,7 +532,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{D5472C9A-2126-4981-9051-1F7DEE252E5F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.31</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>bin</cx:v>
             </cx:txData>
           </cx:tx>
@@ -537,7 +565,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.54</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -548,7 +576,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{DE819021-C758-411F-98B5-86565AFE3C77}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.52</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>num.trees</cx:v>
             </cx:txData>
           </cx:tx>
@@ -580,7 +608,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -591,7 +619,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{186DB5C6-A352-4D50-98D2-A4623FAA88A1}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.9</cx:f>
               <cx:v>max.depth</cx:v>
             </cx:txData>
           </cx:tx>
@@ -623,7 +651,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -634,7 +662,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{56008B2E-B231-48B0-A473-EF124C3145F1}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.3</cx:f>
+              <cx:f>_xlchart.v1.11</cx:f>
               <cx:v>min.node.size</cx:v>
             </cx:txData>
           </cx:tx>
@@ -666,7 +694,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -677,7 +705,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{D6906F87-BE67-4244-A6FE-8BC37984CAA0}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:f>_xlchart.v1.14</cx:f>
               <cx:v>mtry</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4048,8 +4076,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6264274" y="13655675"/>
-              <a:ext cx="4195908" cy="2647950"/>
+              <a:off x="7566024" y="14138275"/>
+              <a:ext cx="4564208" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4126,8 +4154,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6245225" y="16430624"/>
-              <a:ext cx="2443884" cy="4003675"/>
+              <a:off x="7546975" y="17014824"/>
+              <a:ext cx="2812184" cy="4143375"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4204,8 +4232,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10804236" y="13630564"/>
-              <a:ext cx="4555837" cy="2639291"/>
+              <a:off x="12474286" y="14113164"/>
+              <a:ext cx="4555837" cy="2734541"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4282,8 +4310,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="15489238" y="13617575"/>
-              <a:ext cx="4622800" cy="2565400"/>
+              <a:off x="17159288" y="14100175"/>
+              <a:ext cx="4622800" cy="2660650"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4360,8 +4388,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="20246975" y="13554075"/>
-              <a:ext cx="4538134" cy="2722034"/>
+              <a:off x="21917025" y="14036675"/>
+              <a:ext cx="4538134" cy="2817284"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4438,8 +4466,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="25405292" y="13693775"/>
-              <a:ext cx="4572001" cy="2743200"/>
+              <a:off x="26514425" y="14015508"/>
+              <a:ext cx="4538135" cy="2806700"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4769,10 +4797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0927F8-D177-4AA1-A48F-5E921EF2A48F}">
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4846,7 +4874,7 @@
       </c>
       <c r="J2">
         <f>GEOMEAN(I:I)</f>
-        <v>216.76091580646005</v>
+        <v>217.98121884302503</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -6807,7 +6835,7 @@
         <v>66</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I76" si="1">INT(G67/100000)</f>
+        <f t="shared" ref="I67:I98" si="1">INT(G67/100000)</f>
         <v>228</v>
       </c>
     </row>
@@ -7079,6 +7107,666 @@
       <c r="I76">
         <f t="shared" si="1"/>
         <v>218</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>85</v>
+      </c>
+      <c r="B77">
+        <v>954</v>
+      </c>
+      <c r="C77">
+        <v>24</v>
+      </c>
+      <c r="D77">
+        <v>500</v>
+      </c>
+      <c r="E77">
+        <v>26</v>
+      </c>
+      <c r="F77">
+        <v>5</v>
+      </c>
+      <c r="G77" s="1">
+        <v>21854000</v>
+      </c>
+      <c r="H77">
+        <v>77</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="1"/>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78">
+        <v>1643</v>
+      </c>
+      <c r="C78">
+        <v>30</v>
+      </c>
+      <c r="D78">
+        <v>194</v>
+      </c>
+      <c r="E78">
+        <v>2</v>
+      </c>
+      <c r="F78">
+        <v>5</v>
+      </c>
+      <c r="G78" s="1">
+        <v>21586000</v>
+      </c>
+      <c r="H78">
+        <v>78</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="1"/>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79">
+        <v>2496</v>
+      </c>
+      <c r="C79">
+        <v>24</v>
+      </c>
+      <c r="D79">
+        <v>278</v>
+      </c>
+      <c r="E79">
+        <v>10</v>
+      </c>
+      <c r="F79">
+        <v>5</v>
+      </c>
+      <c r="G79" s="1">
+        <v>22480000</v>
+      </c>
+      <c r="H79">
+        <v>79</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="1"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>88</v>
+      </c>
+      <c r="B80">
+        <v>1588</v>
+      </c>
+      <c r="C80">
+        <v>30</v>
+      </c>
+      <c r="D80">
+        <v>176</v>
+      </c>
+      <c r="E80">
+        <v>8</v>
+      </c>
+      <c r="F80">
+        <v>5</v>
+      </c>
+      <c r="G80" s="1">
+        <v>22622000</v>
+      </c>
+      <c r="H80">
+        <v>80</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="1"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>89</v>
+      </c>
+      <c r="B81">
+        <v>1158</v>
+      </c>
+      <c r="C81">
+        <v>23</v>
+      </c>
+      <c r="D81">
+        <v>385</v>
+      </c>
+      <c r="E81">
+        <v>11</v>
+      </c>
+      <c r="F81">
+        <v>5</v>
+      </c>
+      <c r="G81" s="1">
+        <v>22556000</v>
+      </c>
+      <c r="H81">
+        <v>81</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="1"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82">
+        <v>2145</v>
+      </c>
+      <c r="C82">
+        <v>30</v>
+      </c>
+      <c r="D82">
+        <v>217</v>
+      </c>
+      <c r="E82">
+        <v>14</v>
+      </c>
+      <c r="F82">
+        <v>5</v>
+      </c>
+      <c r="G82" s="1">
+        <v>22602000</v>
+      </c>
+      <c r="H82">
+        <v>82</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="1"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>91</v>
+      </c>
+      <c r="B83">
+        <v>2329</v>
+      </c>
+      <c r="C83">
+        <v>20</v>
+      </c>
+      <c r="D83">
+        <v>212</v>
+      </c>
+      <c r="E83">
+        <v>12</v>
+      </c>
+      <c r="F83">
+        <v>5</v>
+      </c>
+      <c r="G83" s="1">
+        <v>22562000</v>
+      </c>
+      <c r="H83">
+        <v>83</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="1"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84">
+        <v>345</v>
+      </c>
+      <c r="C84">
+        <v>30</v>
+      </c>
+      <c r="D84">
+        <v>187</v>
+      </c>
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="F84">
+        <v>5</v>
+      </c>
+      <c r="G84" s="1">
+        <v>21874000</v>
+      </c>
+      <c r="H84">
+        <v>84</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="1"/>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>93</v>
+      </c>
+      <c r="B85">
+        <v>1652</v>
+      </c>
+      <c r="C85">
+        <v>30</v>
+      </c>
+      <c r="D85">
+        <v>203</v>
+      </c>
+      <c r="E85">
+        <v>12</v>
+      </c>
+      <c r="F85">
+        <v>5</v>
+      </c>
+      <c r="G85" s="1">
+        <v>22562000</v>
+      </c>
+      <c r="H85">
+        <v>85</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="1"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86">
+        <v>1881</v>
+      </c>
+      <c r="C86">
+        <v>30</v>
+      </c>
+      <c r="D86">
+        <v>432</v>
+      </c>
+      <c r="E86">
+        <v>12</v>
+      </c>
+      <c r="F86">
+        <v>5</v>
+      </c>
+      <c r="G86" s="1">
+        <v>22382000</v>
+      </c>
+      <c r="H86">
+        <v>86</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="1"/>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>95</v>
+      </c>
+      <c r="B87">
+        <v>2488</v>
+      </c>
+      <c r="C87">
+        <v>29</v>
+      </c>
+      <c r="D87">
+        <v>81</v>
+      </c>
+      <c r="E87">
+        <v>9</v>
+      </c>
+      <c r="F87">
+        <v>5</v>
+      </c>
+      <c r="G87" s="1">
+        <v>22442000</v>
+      </c>
+      <c r="H87">
+        <v>87</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="1"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>96</v>
+      </c>
+      <c r="B88">
+        <v>2496</v>
+      </c>
+      <c r="C88">
+        <v>16</v>
+      </c>
+      <c r="D88">
+        <v>164</v>
+      </c>
+      <c r="E88">
+        <v>10</v>
+      </c>
+      <c r="F88">
+        <v>5</v>
+      </c>
+      <c r="G88" s="1">
+        <v>22494000</v>
+      </c>
+      <c r="H88">
+        <v>88</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="1"/>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>97</v>
+      </c>
+      <c r="B89">
+        <v>1012</v>
+      </c>
+      <c r="C89">
+        <v>23</v>
+      </c>
+      <c r="D89">
+        <v>333</v>
+      </c>
+      <c r="E89">
+        <v>22</v>
+      </c>
+      <c r="F89">
+        <v>5</v>
+      </c>
+      <c r="G89" s="1">
+        <v>22150000</v>
+      </c>
+      <c r="H89">
+        <v>89</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="1"/>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>98</v>
+      </c>
+      <c r="B90">
+        <v>403</v>
+      </c>
+      <c r="C90">
+        <v>30</v>
+      </c>
+      <c r="D90">
+        <v>162</v>
+      </c>
+      <c r="E90">
+        <v>11</v>
+      </c>
+      <c r="F90">
+        <v>5</v>
+      </c>
+      <c r="G90" s="1">
+        <v>22262000</v>
+      </c>
+      <c r="H90">
+        <v>90</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="1"/>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>99</v>
+      </c>
+      <c r="B91">
+        <v>1234</v>
+      </c>
+      <c r="C91">
+        <v>23</v>
+      </c>
+      <c r="D91">
+        <v>228</v>
+      </c>
+      <c r="E91">
+        <v>11</v>
+      </c>
+      <c r="F91">
+        <v>5</v>
+      </c>
+      <c r="G91" s="1">
+        <v>22830000</v>
+      </c>
+      <c r="H91">
+        <v>91</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="1"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>100</v>
+      </c>
+      <c r="B92">
+        <v>1882</v>
+      </c>
+      <c r="C92">
+        <v>10</v>
+      </c>
+      <c r="D92">
+        <v>211</v>
+      </c>
+      <c r="E92">
+        <v>8</v>
+      </c>
+      <c r="F92">
+        <v>5</v>
+      </c>
+      <c r="G92" s="1">
+        <v>21330000</v>
+      </c>
+      <c r="H92">
+        <v>92</v>
+      </c>
+      <c r="I92">
+        <f t="shared" si="1"/>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>101</v>
+      </c>
+      <c r="B93">
+        <v>1500</v>
+      </c>
+      <c r="C93">
+        <v>30</v>
+      </c>
+      <c r="D93">
+        <v>342</v>
+      </c>
+      <c r="E93">
+        <v>11</v>
+      </c>
+      <c r="F93">
+        <v>5</v>
+      </c>
+      <c r="G93" s="1">
+        <v>22330000</v>
+      </c>
+      <c r="H93">
+        <v>93</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="1"/>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>102</v>
+      </c>
+      <c r="B94">
+        <v>2165</v>
+      </c>
+      <c r="C94">
+        <v>30</v>
+      </c>
+      <c r="D94">
+        <v>499</v>
+      </c>
+      <c r="E94">
+        <v>9</v>
+      </c>
+      <c r="F94">
+        <v>5</v>
+      </c>
+      <c r="G94" s="1">
+        <v>22562000</v>
+      </c>
+      <c r="H94">
+        <v>94</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="1"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>103</v>
+      </c>
+      <c r="B95">
+        <v>2119</v>
+      </c>
+      <c r="C95">
+        <v>16</v>
+      </c>
+      <c r="D95">
+        <v>255</v>
+      </c>
+      <c r="E95">
+        <v>11</v>
+      </c>
+      <c r="F95">
+        <v>5</v>
+      </c>
+      <c r="G95" s="1">
+        <v>22680000</v>
+      </c>
+      <c r="H95">
+        <v>95</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="1"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>104</v>
+      </c>
+      <c r="B96">
+        <v>746</v>
+      </c>
+      <c r="C96">
+        <v>25</v>
+      </c>
+      <c r="D96">
+        <v>377</v>
+      </c>
+      <c r="E96">
+        <v>15</v>
+      </c>
+      <c r="F96">
+        <v>5</v>
+      </c>
+      <c r="G96" s="1">
+        <v>22202000</v>
+      </c>
+      <c r="H96">
+        <v>96</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="1"/>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>105</v>
+      </c>
+      <c r="B97">
+        <v>300</v>
+      </c>
+      <c r="C97">
+        <v>19</v>
+      </c>
+      <c r="D97">
+        <v>401</v>
+      </c>
+      <c r="E97">
+        <v>23</v>
+      </c>
+      <c r="F97">
+        <v>5</v>
+      </c>
+      <c r="G97" s="1">
+        <v>21772000</v>
+      </c>
+      <c r="H97">
+        <v>97</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="1"/>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>106</v>
+      </c>
+      <c r="B98">
+        <v>1325</v>
+      </c>
+      <c r="C98">
+        <v>21</v>
+      </c>
+      <c r="D98">
+        <v>257</v>
+      </c>
+      <c r="E98">
+        <v>21</v>
+      </c>
+      <c r="F98">
+        <v>5</v>
+      </c>
+      <c r="G98" s="1">
+        <v>21968000</v>
+      </c>
+      <c r="H98">
+        <v>98</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="1"/>
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>